<commit_message>
Updated excel data to new week
</commit_message>
<xml_diff>
--- a/data/filter_data.xlsx
+++ b/data/filter_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26704"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9D73174-9854-4210-87BE-A0F88234698B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95F17C53-5C50-4525-ADAB-7BD48361278C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,7 +570,7 @@
         <v>16</v>
       </c>
       <c r="F5">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:6">

</xml_diff>